<commit_message>
restructure the data folders
</commit_message>
<xml_diff>
--- a/code/20191021.xlsx
+++ b/code/20191021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewhu/Desktop/Graduate-project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA0FC72-6660-D54D-B82D-13F44AB68412}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E416382-0643-284D-9AB4-4F99602454A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="單向當沖基本統計量" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="稅率調降基本統計量(半年)" sheetId="4" r:id="rId4"/>
     <sheet name="稅率調降基本統計量(一年)" sheetId="5" r:id="rId5"/>
     <sheet name="基本統計量檢定結果" sheetId="6" r:id="rId6"/>
-    <sheet name="Part 3" sheetId="7" r:id="rId7"/>
-    <sheet name="Correlation" sheetId="8" r:id="rId8"/>
+    <sheet name="Δy顯著性結果" sheetId="7" r:id="rId7"/>
+    <sheet name="相關係數" sheetId="8" r:id="rId8"/>
+    <sheet name="迴歸" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -7583,18 +7584,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="I18:O18"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="I33:O33"/>
+    <mergeCell ref="B32:O32"/>
+    <mergeCell ref="A31:O31"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="I3:O3"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B17:O17"/>
     <mergeCell ref="A16:O16"/>
-    <mergeCell ref="I18:O18"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="I33:O33"/>
-    <mergeCell ref="B32:O32"/>
-    <mergeCell ref="A31:O31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -9157,6 +9158,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B32:O32"/>
+    <mergeCell ref="I33:O33"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="A31:O31"/>
+    <mergeCell ref="B3:H3"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="I3:O3"/>
@@ -9164,11 +9170,6 @@
     <mergeCell ref="I18:O18"/>
     <mergeCell ref="A16:O16"/>
     <mergeCell ref="B17:O17"/>
-    <mergeCell ref="B32:O32"/>
-    <mergeCell ref="I33:O33"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="A31:O31"/>
-    <mergeCell ref="B3:H3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -13850,12 +13851,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="A29:P29"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="B30:D30"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="H16:J16"/>
@@ -13868,6 +13863,12 @@
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="E2:G2"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="A29:P29"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="B30:D30"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -13878,7 +13879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
@@ -15301,24 +15302,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="A14:P14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="N15:P15"/>
     <mergeCell ref="A27:P27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="E28:G28"/>
     <mergeCell ref="H28:J28"/>
     <mergeCell ref="K28:M28"/>
     <mergeCell ref="N28:P28"/>
-    <mergeCell ref="A14:P14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15538,4 +15539,16 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82B35C8-723F-654E-9C75-434AEF6E85A5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>